<commit_message>
finihsed step 2B in excel sheet
</commit_message>
<xml_diff>
--- a/01_project-steps-delivering-an-ml-ai-strategy.xlsx
+++ b/01_project-steps-delivering-an-ml-ai-strategy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDriveSysncOsa\OneDrive - Taibah University\DropBox\1440-1441 Second Semester\Udacity Reviewer\My own projects\ML Project\Github Repo\Delivering-an-ML-AI-Strategy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{F6D73E04-F98F-4F45-82A3-AB2F1AC194F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9E427180-D723-4303-9F62-3303CC4C6B79}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="13_ncr:1_{F6D73E04-F98F-4F45-82A3-AB2F1AC194F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CAB5FA55-28F4-4479-A901-97D01CCE0C6C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="9" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="15" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIRECTIONS" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="333">
   <si>
     <t>Step 0: Choose Your Business Context</t>
   </si>
@@ -1547,6 +1547,9 @@
   </si>
   <si>
     <t>machine learning is forcing inspection’s inflection point across supply chains today</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -16426,7 +16429,7 @@
   </sheetPr>
   <dimension ref="A1:K1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
@@ -19558,7 +19561,9 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -19605,7 +19610,9 @@
         <f>'Step 1A - UC 1'!D15</f>
         <v>resolution</v>
       </c>
-      <c r="E4" s="50"/>
+      <c r="E4" s="50" t="s">
+        <v>332</v>
+      </c>
       <c r="F4" s="43" t="s">
         <v>118</v>
       </c>
@@ -19658,7 +19665,9 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -19705,7 +19714,9 @@
         <f>'Step 1A - UC 2'!D15</f>
         <v>resolution</v>
       </c>
-      <c r="E4" s="50"/>
+      <c r="E4" s="50" t="s">
+        <v>332</v>
+      </c>
       <c r="F4" s="43" t="s">
         <v>118</v>
       </c>
@@ -19719,7 +19730,9 @@
         <f>'Step 1A - UC 2'!D9</f>
         <v>0</v>
       </c>
-      <c r="E5" s="44"/>
+      <c r="E5" s="44" t="s">
+        <v>332</v>
+      </c>
       <c r="F5" s="43" t="s">
         <v>119</v>
       </c>
@@ -19872,7 +19885,9 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -19919,7 +19934,9 @@
         <f>'Step 1A - UC 3'!D15</f>
         <v>resolution</v>
       </c>
-      <c r="E4" s="50"/>
+      <c r="E4" s="50" t="s">
+        <v>332</v>
+      </c>
       <c r="F4" s="43" t="s">
         <v>118</v>
       </c>
@@ -19945,7 +19962,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1">
-      <c r="E7" s="44"/>
+      <c r="E7" s="44" t="s">
+        <v>332</v>
+      </c>
       <c r="F7" s="43" t="s">
         <v>121</v>
       </c>
@@ -19978,7 +19997,9 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -20039,7 +20060,9 @@
         <f>'Step 1A - UC 4'!D9</f>
         <v>0</v>
       </c>
-      <c r="E5" s="44"/>
+      <c r="E5" s="44" t="s">
+        <v>332</v>
+      </c>
       <c r="F5" s="43" t="s">
         <v>119</v>
       </c>
@@ -20084,7 +20107,9 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -20145,7 +20170,9 @@
         <f>'Step 1A - UC 5'!D9</f>
         <v>0</v>
       </c>
-      <c r="E5" s="44"/>
+      <c r="E5" s="44" t="s">
+        <v>332</v>
+      </c>
       <c r="F5" s="43" t="s">
         <v>119</v>
       </c>
@@ -20190,7 +20217,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>

</xml_diff>

<commit_message>
completed Step 3 of the project
</commit_message>
<xml_diff>
--- a/01_project-steps-delivering-an-ml-ai-strategy.xlsx
+++ b/01_project-steps-delivering-an-ml-ai-strategy.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="134" documentId="13_ncr:1_{F6D73E04-F98F-4F45-82A3-AB2F1AC194F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CAB5FA55-28F4-4479-A901-97D01CCE0C6C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="15" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIRECTIONS" sheetId="1" r:id="rId1"/>
@@ -3515,8 +3515,8 @@
   </sheetPr>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -20217,7 +20217,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
@@ -39400,7 +39400,7 @@
   <dimension ref="A1:AA1005"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B9" sqref="B9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
finished up to step 5
</commit_message>
<xml_diff>
--- a/01_project-steps-delivering-an-ml-ai-strategy.xlsx
+++ b/01_project-steps-delivering-an-ml-ai-strategy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDriveSysncOsa\OneDrive - Taibah University\DropBox\1440-1441 Second Semester\Udacity Reviewer\My own projects\ML Project\Github Repo\Delivering-an-ML-AI-Strategy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="13_ncr:1_{F6D73E04-F98F-4F45-82A3-AB2F1AC194F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CAB5FA55-28F4-4479-A901-97D01CCE0C6C}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="13_ncr:1_{F6D73E04-F98F-4F45-82A3-AB2F1AC194F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{227EAD98-543B-4A12-8C86-60E586E615FA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="22" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIRECTIONS" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="334">
   <si>
     <t>Step 0: Choose Your Business Context</t>
   </si>
@@ -1550,6 +1550,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -3515,7 +3518,7 @@
   </sheetPr>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -20261,7 +20264,9 @@
   </sheetPr>
   <dimension ref="A1:AB1005"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="D113" sqref="D113"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -20438,7 +20443,9 @@
       </c>
       <c r="B12" s="62"/>
       <c r="C12" s="62"/>
-      <c r="D12" s="63"/>
+      <c r="D12" s="63" t="s">
+        <v>333</v>
+      </c>
       <c r="E12" s="64"/>
       <c r="F12" s="64"/>
       <c r="G12" s="64"/>
@@ -20472,7 +20479,9 @@
       <c r="C13" s="66" t="s">
         <v>134</v>
       </c>
-      <c r="D13" s="56"/>
+      <c r="D13" s="56">
+        <v>4</v>
+      </c>
       <c r="E13" s="66" t="s">
         <v>135</v>
       </c>
@@ -20481,25 +20490,33 @@
       <c r="A14" s="65" t="s">
         <v>141</v>
       </c>
-      <c r="D14" s="56"/>
+      <c r="D14" s="56">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:28" ht="30">
       <c r="A15" s="59" t="s">
         <v>137</v>
       </c>
-      <c r="D15" s="56"/>
+      <c r="D15" s="56">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:28" ht="45">
       <c r="A16" s="59" t="s">
         <v>138</v>
       </c>
-      <c r="D16" s="56"/>
+      <c r="D16" s="56">
+        <v>4</v>
+      </c>
     </row>
     <row r="17" spans="1:28" ht="30">
       <c r="A17" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="D17" s="56"/>
+      <c r="D17" s="56">
+        <v>5</v>
+      </c>
     </row>
     <row r="18" spans="1:28" ht="15.75" customHeight="1">
       <c r="A18" s="61" t="s">
@@ -21542,7 +21559,9 @@
       </c>
       <c r="B108" s="64"/>
       <c r="C108" s="64"/>
-      <c r="D108" s="63"/>
+      <c r="D108" s="63" t="s">
+        <v>333</v>
+      </c>
       <c r="E108" s="64"/>
       <c r="F108" s="64"/>
       <c r="G108" s="64"/>
@@ -21576,7 +21595,9 @@
       <c r="C109" s="66" t="s">
         <v>134</v>
       </c>
-      <c r="D109" s="56"/>
+      <c r="D109" s="56">
+        <v>5</v>
+      </c>
       <c r="E109" s="66" t="s">
         <v>135</v>
       </c>
@@ -21585,25 +21606,33 @@
       <c r="A110" s="68" t="s">
         <v>226</v>
       </c>
-      <c r="D110" s="56"/>
+      <c r="D110" s="56">
+        <v>5</v>
+      </c>
     </row>
     <row r="111" spans="1:28" ht="30">
       <c r="A111" s="68" t="s">
         <v>227</v>
       </c>
-      <c r="D111" s="56"/>
+      <c r="D111" s="56">
+        <v>5</v>
+      </c>
     </row>
     <row r="112" spans="1:28" ht="30">
       <c r="A112" s="68" t="s">
         <v>228</v>
       </c>
-      <c r="D112" s="56"/>
+      <c r="D112" s="56">
+        <v>5</v>
+      </c>
     </row>
     <row r="113" spans="1:4" ht="45">
       <c r="A113" s="68" t="s">
         <v>229</v>
       </c>
-      <c r="D113" s="56"/>
+      <c r="D113" s="56">
+        <v>5</v>
+      </c>
     </row>
     <row r="114" spans="1:4" ht="12.75">
       <c r="D114" s="56"/>
@@ -24413,7 +24442,9 @@
   </sheetPr>
   <dimension ref="A1:AB1005"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="E104" sqref="E104"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -24592,7 +24623,9 @@
       </c>
       <c r="B12" s="62"/>
       <c r="C12" s="62"/>
-      <c r="D12" s="63"/>
+      <c r="D12" s="63" t="s">
+        <v>333</v>
+      </c>
       <c r="E12" s="64"/>
       <c r="F12" s="64"/>
       <c r="G12" s="64"/>
@@ -24626,7 +24659,9 @@
       <c r="C13" s="66" t="s">
         <v>134</v>
       </c>
-      <c r="D13" s="56"/>
+      <c r="D13" s="56">
+        <v>4</v>
+      </c>
       <c r="E13" s="66" t="s">
         <v>135</v>
       </c>
@@ -24635,25 +24670,33 @@
       <c r="A14" s="65" t="s">
         <v>141</v>
       </c>
-      <c r="D14" s="56"/>
+      <c r="D14" s="56">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:28" ht="30">
       <c r="A15" s="59" t="s">
         <v>137</v>
       </c>
-      <c r="D15" s="56"/>
+      <c r="D15" s="56">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:28" ht="45">
       <c r="A16" s="59" t="s">
         <v>138</v>
       </c>
-      <c r="D16" s="56"/>
+      <c r="D16" s="56">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:28" ht="30">
       <c r="A17" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="D17" s="56"/>
+      <c r="D17" s="56">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" spans="1:28" ht="15.75" customHeight="1">
       <c r="A18" s="61" t="s">
@@ -25568,7 +25611,9 @@
       </c>
       <c r="B96" s="64"/>
       <c r="C96" s="64"/>
-      <c r="D96" s="63"/>
+      <c r="D96" s="63" t="s">
+        <v>333</v>
+      </c>
       <c r="E96" s="64"/>
       <c r="F96" s="64"/>
       <c r="G96" s="64"/>
@@ -25602,7 +25647,9 @@
       <c r="C97" s="66" t="s">
         <v>134</v>
       </c>
-      <c r="D97" s="58"/>
+      <c r="D97" s="58">
+        <v>3</v>
+      </c>
       <c r="E97" s="66" t="s">
         <v>135</v>
       </c>
@@ -25611,25 +25658,33 @@
       <c r="A98" s="65" t="s">
         <v>217</v>
       </c>
-      <c r="D98" s="58"/>
+      <c r="D98" s="58">
+        <v>4</v>
+      </c>
     </row>
     <row r="99" spans="1:28" ht="30">
       <c r="A99" s="59" t="s">
         <v>218</v>
       </c>
-      <c r="D99" s="58"/>
+      <c r="D99" s="58">
+        <v>3</v>
+      </c>
     </row>
     <row r="100" spans="1:28" ht="30">
       <c r="A100" s="59" t="s">
         <v>208</v>
       </c>
-      <c r="D100" s="58"/>
+      <c r="D100" s="58">
+        <v>3</v>
+      </c>
     </row>
     <row r="101" spans="1:28" ht="45">
       <c r="A101" s="59" t="s">
         <v>219</v>
       </c>
-      <c r="D101" s="58"/>
+      <c r="D101" s="58">
+        <v>3</v>
+      </c>
     </row>
     <row r="102" spans="1:28">
       <c r="A102" s="61" t="s">
@@ -28576,7 +28631,9 @@
   </sheetPr>
   <dimension ref="A1:J113"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -28640,7 +28697,9 @@
       </c>
       <c r="B6" s="62"/>
       <c r="C6" s="62"/>
-      <c r="D6" s="63"/>
+      <c r="D6" s="63" t="s">
+        <v>333</v>
+      </c>
       <c r="E6" s="64"/>
       <c r="F6" s="64"/>
       <c r="G6" s="64"/>
@@ -28656,7 +28715,9 @@
       <c r="C7" s="66" t="s">
         <v>134</v>
       </c>
-      <c r="D7" s="56"/>
+      <c r="D7" s="56">
+        <v>5</v>
+      </c>
       <c r="E7" s="66" t="s">
         <v>135</v>
       </c>
@@ -28667,7 +28728,9 @@
       </c>
       <c r="B8" s="52"/>
       <c r="C8" s="52"/>
-      <c r="D8" s="56"/>
+      <c r="D8" s="56">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="30">
       <c r="A9" s="59" t="s">
@@ -28675,7 +28738,9 @@
       </c>
       <c r="B9" s="52"/>
       <c r="C9" s="52"/>
-      <c r="D9" s="56"/>
+      <c r="D9" s="56">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="45">
       <c r="A10" s="59" t="s">
@@ -28683,7 +28748,9 @@
       </c>
       <c r="B10" s="52"/>
       <c r="C10" s="52"/>
-      <c r="D10" s="56"/>
+      <c r="D10" s="56">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="30">
       <c r="A11" s="59" t="s">
@@ -28691,7 +28758,9 @@
       </c>
       <c r="B11" s="52"/>
       <c r="C11" s="52"/>
-      <c r="D11" s="56"/>
+      <c r="D11" s="56">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1">
       <c r="A12" s="61" t="s">
@@ -29752,17 +29821,17 @@
       </c>
       <c r="C9" s="38">
         <f>COUNTIF('Step 4A - one UC'!D6:D108, "y")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9" s="38"/>
       <c r="E9" s="38">
         <f>COUNTIF('Step 4A - a second UC'!D6:D108, "y")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" s="38"/>
       <c r="G9" s="38">
         <f>COUNTIF('Step 4A - a third UC'!D6:D108, "y")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1">
@@ -29771,17 +29840,17 @@
       </c>
       <c r="C10" s="38">
         <f>SUM('Step 4A - one UC'!D:D)</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="38">
         <f>SUM('Step 4A - a second UC'!D:D)</f>
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="38">
         <f>SUM('Step 4A - a third UC'!D:D)</f>
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1">
@@ -29790,36 +29859,36 @@
       </c>
       <c r="C11" s="38">
         <f>C9*5*5</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="38">
         <f>E9*5*5</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="38">
         <f>G9*5*5</f>
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1">
       <c r="A12" s="70" t="s">
         <v>238</v>
       </c>
-      <c r="C12" s="71" t="e">
+      <c r="C12" s="71">
         <f>(C10/C11)*100</f>
-        <v>#DIV/0!</v>
+        <v>94</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="71" t="e">
+      <c r="E12" s="71">
         <f>(E10/E11)*100</f>
-        <v>#DIV/0!</v>
+        <v>112.00000000000001</v>
       </c>
       <c r="F12" s="5"/>
-      <c r="G12" s="71" t="e">
+      <c r="G12" s="71">
         <f>(G10/G11)*100</f>
-        <v>#DIV/0!</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1">
@@ -30068,7 +30137,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>

</xml_diff>

<commit_message>
completed the final report
</commit_message>
<xml_diff>
--- a/01_project-steps-delivering-an-ml-ai-strategy.xlsx
+++ b/01_project-steps-delivering-an-ml-ai-strategy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDriveSysncOsa\OneDrive - Taibah University\DropBox\1440-1441 Second Semester\Udacity Reviewer\My own projects\ML Project\Github Repo\Delivering-an-ML-AI-Strategy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="184" documentId="13_ncr:1_{F6D73E04-F98F-4F45-82A3-AB2F1AC194F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{227EAD98-543B-4A12-8C86-60E586E615FA}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="13_ncr:1_{F6D73E04-F98F-4F45-82A3-AB2F1AC194F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AF1D3BA8-1E59-4382-A6EE-49E50C1E1980}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="22" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIRECTIONS" sheetId="1" r:id="rId1"/>
@@ -3518,8 +3518,8 @@
   </sheetPr>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -30137,7 +30137,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
@@ -30160,7 +30160,7 @@
   <dimension ref="A1:E1012"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B9" sqref="B9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -33293,7 +33293,7 @@
   <dimension ref="A1:AA1005"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -45645,7 +45645,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
updated use cases in the excel sheet
</commit_message>
<xml_diff>
--- a/01_project-steps-delivering-an-ml-ai-strategy.xlsx
+++ b/01_project-steps-delivering-an-ml-ai-strategy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDriveSysncOsa\OneDrive - Taibah University\DropBox\1440-1441 Second Semester\Udacity Reviewer\My own projects\ML Project\Github Repo\Delivering-an-ML-AI-Strategy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="13_ncr:1_{F6D73E04-F98F-4F45-82A3-AB2F1AC194F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AF1D3BA8-1E59-4382-A6EE-49E50C1E1980}"/>
+  <xr:revisionPtr revIDLastSave="210" documentId="13_ncr:1_{F6D73E04-F98F-4F45-82A3-AB2F1AC194F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BDD66B35-4768-4884-AE77-1CB0E1270B05}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIRECTIONS" sheetId="1" r:id="rId1"/>
@@ -1297,30 +1297,6 @@
     <t>(Quality Control with Computer Vision )</t>
   </si>
   <si>
-    <t>collecting random samples</t>
-  </si>
-  <si>
-    <t>more increase in random samples</t>
-  </si>
-  <si>
-    <t>stop machine / line</t>
-  </si>
-  <si>
-    <t>The entire dataset will be explored instead of random sample</t>
-  </si>
-  <si>
-    <t>The devices will be checked using CV to check if it is defective or not</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if number of defective devices &gt; threshold </t>
-  </si>
-  <si>
-    <t>stop machine /line. The accuracy if very hight the machine/line will be stopped only if there are defectives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if number of defectives in the random sample  &gt; threshold </t>
-  </si>
-  <si>
     <t>(Optimal tax strategy predictor)</t>
   </si>
   <si>
@@ -1349,30 +1325,6 @@
   </si>
   <si>
     <t>(Car Detection of Customer ID)</t>
-  </si>
-  <si>
-    <t>The car preferences</t>
-  </si>
-  <si>
-    <t>The customer should change it manually</t>
-  </si>
-  <si>
-    <t>In case the customer find uncomfortable thing, he shall do it manually</t>
-  </si>
-  <si>
-    <t>Customer service may help him in changing preferences manually</t>
-  </si>
-  <si>
-    <t>car preferences are collected</t>
-  </si>
-  <si>
-    <t>we should join preferences to each corresponding customer id</t>
-  </si>
-  <si>
-    <t>Camera can detect the customer face to define the customer id</t>
-  </si>
-  <si>
-    <t>car preferences are changed automatically</t>
   </si>
   <si>
     <t>(Car Maintenance Expector)</t>
@@ -1553,6 +1505,60 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">samples of defective devices
+- general categories of defectives. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">defectives are categoriezed according to urgency. 
+- some defective types may lead to pausing production line. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">search if number of defective devices passing the production line is &gt; threshold or the defective urgency is high </t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of defectives may lead to pausing or stopping production line. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">camera is focused on products on the production line. Camera collects samples of defective and non-defective devices. 
+- historical products data in both defective and non-defective states are collected. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the list of collected historical images of defective and non-defective devices are used in training AI classifier </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The trained model classifier are used in real time classification through camera to classify each product as eigher defective or non-defective and also measure its defective urgency. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">high defective productes thershold may stop or pause the production line. Git rid of the defective product. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The collected user images will be used to "re-train" the model on the new user's dataset. </t>
+  </si>
+  <si>
+    <t>pr-trained models for face recognition 
+- collect user face images with different angles and shapes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The trained model will detect the customer face with approximately 4% False Negatives. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The car will respond, opening locks, flash signs, etc. </t>
+  </si>
+  <si>
+    <t>key with sensor
+- the sensor has something like code that transferred wirelessly</t>
+  </si>
+  <si>
+    <t>car has also receiving device that only unlock when spcific code is received</t>
+  </si>
+  <si>
+    <t>The car is programmed to accept spcific wireless code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the code detected, the car responds accordingly, opening door lock, signals, etc. </t>
   </si>
 </sst>
 </file>
@@ -3383,19 +3389,20 @@
       </c>
       <c r="C8" s="28" t="str">
         <f>'Step 1A - UC 3'!B14</f>
-        <v>car preferences are collected</v>
+        <v>pr-trained models for face recognition 
+- collect user face images with different angles and shapes</v>
       </c>
       <c r="D8" s="28" t="str">
         <f>'Step 1A - UC 3'!C14</f>
-        <v>we should join preferences to each corresponding customer id</v>
+        <v xml:space="preserve">The collected user images will be used to "re-train" the model on the new user's dataset. </v>
       </c>
       <c r="E8" s="28" t="str">
         <f>'Step 1A - UC 3'!D14</f>
-        <v>Camera can detect the customer face to define the customer id</v>
+        <v xml:space="preserve">The trained model will detect the customer face with approximately 4% False Negatives. </v>
       </c>
       <c r="F8" s="28" t="str">
         <f>'Step 1A - UC 3'!E14</f>
-        <v>car preferences are changed automatically</v>
+        <v xml:space="preserve">The car will respond, opening locks, flash signs, etc. </v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15">
@@ -3424,7 +3431,7 @@
         <v>52</v>
       </c>
       <c r="D13" s="82" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -3433,7 +3440,7 @@
         <v>53</v>
       </c>
       <c r="D14" s="82" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15">
@@ -3441,7 +3448,7 @@
         <v>54</v>
       </c>
       <c r="D15" s="82" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="15">
@@ -3452,7 +3459,7 @@
         <v>56</v>
       </c>
       <c r="D17" s="83" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="15">
@@ -3460,7 +3467,7 @@
         <v>57</v>
       </c>
       <c r="D18" s="83" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="15">
@@ -3468,7 +3475,7 @@
         <v>58</v>
       </c>
       <c r="D19" s="83" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="15">
@@ -3476,7 +3483,7 @@
         <v>59</v>
       </c>
       <c r="D20" s="83" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="15">
@@ -3484,7 +3491,7 @@
         <v>60</v>
       </c>
       <c r="D21" s="83" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15">
@@ -3518,7 +3525,7 @@
   </sheetPr>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D17" sqref="D17:D21"/>
     </sheetView>
   </sheetViews>
@@ -3613,7 +3620,7 @@
         <v>52</v>
       </c>
       <c r="D13" s="82" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -3622,7 +3629,7 @@
         <v>53</v>
       </c>
       <c r="D14" s="82" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15">
@@ -3630,7 +3637,7 @@
         <v>54</v>
       </c>
       <c r="D15" s="82" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="15">
@@ -3641,7 +3648,7 @@
         <v>56</v>
       </c>
       <c r="D17" s="83" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="15">
@@ -3649,7 +3656,7 @@
         <v>57</v>
       </c>
       <c r="D18" s="81" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="15">
@@ -3657,7 +3664,7 @@
         <v>58</v>
       </c>
       <c r="D19" s="81" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="15">
@@ -3665,7 +3672,7 @@
         <v>59</v>
       </c>
       <c r="D20" s="81" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="15">
@@ -3673,7 +3680,7 @@
         <v>60</v>
       </c>
       <c r="D21" s="81" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15">
@@ -3802,7 +3809,7 @@
         <v>52</v>
       </c>
       <c r="D13" s="82" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -3811,7 +3818,7 @@
         <v>53</v>
       </c>
       <c r="D14" s="82" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15">
@@ -3819,7 +3826,7 @@
         <v>54</v>
       </c>
       <c r="D15" s="82" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="15">
@@ -3830,7 +3837,7 @@
         <v>56</v>
       </c>
       <c r="D17" s="81" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="15">
@@ -3838,7 +3845,7 @@
         <v>57</v>
       </c>
       <c r="D18" s="81" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="15">
@@ -3846,7 +3853,7 @@
         <v>58</v>
       </c>
       <c r="D19" s="81" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="15">
@@ -3854,7 +3861,7 @@
         <v>59</v>
       </c>
       <c r="D20" s="81" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="15">
@@ -3862,7 +3869,7 @@
         <v>60</v>
       </c>
       <c r="D21" s="81" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15">
@@ -3931,7 +3938,8 @@
     <row r="3" spans="1:11" ht="15.75" customHeight="1">
       <c r="B3" s="42" t="str">
         <f>'Step 1A - UC 1'!B14</f>
-        <v>The entire dataset will be explored instead of random sample</v>
+        <v xml:space="preserve">camera is focused on products on the production line. Camera collects samples of defective and non-defective devices. 
+- historical products data in both defective and non-defective states are collected. </v>
       </c>
       <c r="D3" s="43" t="s">
         <v>77</v>
@@ -10195,7 +10203,8 @@
     <row r="3" spans="1:11" ht="15.75" customHeight="1">
       <c r="B3" s="41" t="str">
         <f>'Step 1A - UC 3'!B14</f>
-        <v>car preferences are collected</v>
+        <v>pr-trained models for face recognition 
+- collect user face images with different angles and shapes</v>
       </c>
       <c r="D3" s="43" t="s">
         <v>76</v>
@@ -19596,11 +19605,11 @@
     <row r="3" spans="1:8" ht="15.75" customHeight="1">
       <c r="B3" s="47" t="str">
         <f>'Step 1A - UC 1'!C14</f>
-        <v>The devices will be checked using CV to check if it is defective or not</v>
+        <v xml:space="preserve">the list of collected historical images of defective and non-defective devices are used in training AI classifier </v>
       </c>
       <c r="C3" s="47" t="str">
         <f>'Step 1A - UC 1'!D14</f>
-        <v xml:space="preserve">if number of defective devices &gt; threshold </v>
+        <v xml:space="preserve">The trained model classifier are used in real time classification through camera to classify each product as eigher defective or non-defective and also measure its defective urgency. </v>
       </c>
       <c r="E3" s="48"/>
     </row>
@@ -19614,7 +19623,7 @@
         <v>resolution</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="F4" s="43" t="s">
         <v>118</v>
@@ -19718,7 +19727,7 @@
         <v>resolution</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="F4" s="43" t="s">
         <v>118</v>
@@ -19734,7 +19743,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="F5" s="43" t="s">
         <v>119</v>
@@ -19920,11 +19929,11 @@
     <row r="3" spans="1:8" ht="15.75" customHeight="1">
       <c r="B3" s="47" t="str">
         <f>'Step 1A - UC 3'!C14</f>
-        <v>we should join preferences to each corresponding customer id</v>
+        <v xml:space="preserve">The collected user images will be used to "re-train" the model on the new user's dataset. </v>
       </c>
       <c r="C3" s="47" t="str">
         <f>'Step 1A - UC 3'!D14</f>
-        <v>Camera can detect the customer face to define the customer id</v>
+        <v xml:space="preserve">The trained model will detect the customer face with approximately 4% False Negatives. </v>
       </c>
       <c r="E3" s="48"/>
     </row>
@@ -19938,7 +19947,7 @@
         <v>resolution</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="F4" s="43" t="s">
         <v>118</v>
@@ -19966,7 +19975,7 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1">
       <c r="E7" s="44" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="F7" s="43" t="s">
         <v>121</v>
@@ -20064,7 +20073,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="F5" s="43" t="s">
         <v>119</v>
@@ -20174,7 +20183,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="F5" s="43" t="s">
         <v>119</v>
@@ -20444,7 +20453,7 @@
       <c r="B12" s="62"/>
       <c r="C12" s="62"/>
       <c r="D12" s="63" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="E12" s="64"/>
       <c r="F12" s="64"/>
@@ -21560,7 +21569,7 @@
       <c r="B108" s="64"/>
       <c r="C108" s="64"/>
       <c r="D108" s="63" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="E108" s="64"/>
       <c r="F108" s="64"/>
@@ -24624,7 +24633,7 @@
       <c r="B12" s="62"/>
       <c r="C12" s="62"/>
       <c r="D12" s="63" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="E12" s="64"/>
       <c r="F12" s="64"/>
@@ -25612,7 +25621,7 @@
       <c r="B96" s="64"/>
       <c r="C96" s="64"/>
       <c r="D96" s="63" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="E96" s="64"/>
       <c r="F96" s="64"/>
@@ -28698,7 +28707,7 @@
       <c r="B6" s="62"/>
       <c r="C6" s="62"/>
       <c r="D6" s="63" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="E6" s="64"/>
       <c r="F6" s="64"/>
@@ -30159,8 +30168,8 @@
   </sheetPr>
   <dimension ref="A1:E1012"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:E9"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -30249,21 +30258,21 @@
       <c r="D9" s="85"/>
       <c r="E9" s="85"/>
     </row>
-    <row r="10" spans="1:5" ht="36">
+    <row r="10" spans="1:5" ht="90">
       <c r="A10" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="80" t="s">
-        <v>248</v>
+        <v>318</v>
       </c>
       <c r="C10" s="80" t="s">
-        <v>249</v>
+        <v>319</v>
       </c>
       <c r="D10" s="80" t="s">
-        <v>255</v>
+        <v>320</v>
       </c>
       <c r="E10" s="80" t="s">
-        <v>250</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15">
@@ -30305,18 +30314,18 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="66" customHeight="1">
+    <row r="14" spans="1:5" ht="123.75" customHeight="1">
       <c r="B14" s="80" t="s">
-        <v>251</v>
+        <v>322</v>
       </c>
       <c r="C14" s="80" t="s">
-        <v>252</v>
+        <v>323</v>
       </c>
       <c r="D14" s="80" t="s">
-        <v>253</v>
+        <v>324</v>
       </c>
       <c r="E14" s="80" t="s">
-        <v>254</v>
+        <v>325</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15">
@@ -33293,7 +33302,7 @@
   <dimension ref="A1:AA1005"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -33398,7 +33407,7 @@
     </row>
     <row r="9" spans="1:27" ht="42" customHeight="1">
       <c r="B9" s="86" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C9" s="85"/>
       <c r="D9" s="85"/>
@@ -33431,16 +33440,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15">
@@ -33484,16 +33493,16 @@
     </row>
     <row r="14" spans="1:27" ht="60" customHeight="1">
       <c r="B14" s="13" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="15">
@@ -36381,7 +36390,7 @@
   <dimension ref="A1:AA1005"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -36486,7 +36495,7 @@
     </row>
     <row r="9" spans="1:27" ht="34.5" customHeight="1">
       <c r="B9" s="86" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="C9" s="85"/>
       <c r="D9" s="85"/>
@@ -36514,21 +36523,21 @@
       <c r="Z9" s="24"/>
       <c r="AA9" s="24"/>
     </row>
-    <row r="10" spans="1:27" ht="45">
+    <row r="10" spans="1:27" ht="60">
       <c r="A10" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>266</v>
+        <v>330</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>267</v>
+        <v>331</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>268</v>
+        <v>332</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15">
@@ -36570,18 +36579,18 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="51" customHeight="1">
+    <row r="14" spans="1:27" ht="84" customHeight="1">
       <c r="B14" s="13" t="s">
-        <v>270</v>
+        <v>327</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>271</v>
+        <v>326</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>272</v>
+        <v>328</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>273</v>
+        <v>329</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="15">
@@ -39468,7 +39477,7 @@
   </sheetPr>
   <dimension ref="A1:AA1005"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9:E9"/>
     </sheetView>
   </sheetViews>
@@ -39574,7 +39583,7 @@
     </row>
     <row r="9" spans="1:27" ht="74.25" customHeight="1">
       <c r="B9" s="86" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="C9" s="85"/>
       <c r="D9" s="85"/>
@@ -39607,16 +39616,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15">
@@ -39660,16 +39669,16 @@
     </row>
     <row r="14" spans="1:27" ht="35.25" customHeight="1">
       <c r="B14" s="13" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="15">
@@ -42557,7 +42566,7 @@
   <dimension ref="A1:AA1006"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B9" sqref="B9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -42662,7 +42671,7 @@
     </row>
     <row r="9" spans="1:27" ht="37.5" customHeight="1">
       <c r="B9" s="86" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
       <c r="C9" s="85"/>
       <c r="D9" s="85"/>
@@ -42695,16 +42704,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15">
@@ -42748,16 +42757,16 @@
     </row>
     <row r="14" spans="1:27" ht="35.25" customHeight="1">
       <c r="B14" s="13" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="15">
@@ -45698,19 +45707,20 @@
       </c>
       <c r="C8" s="28" t="str">
         <f>'Step 1A - UC 1'!B14</f>
-        <v>The entire dataset will be explored instead of random sample</v>
+        <v xml:space="preserve">camera is focused on products on the production line. Camera collects samples of defective and non-defective devices. 
+- historical products data in both defective and non-defective states are collected. </v>
       </c>
       <c r="D8" s="28" t="str">
         <f>'Step 1A - UC 1'!C14</f>
-        <v>The devices will be checked using CV to check if it is defective or not</v>
+        <v xml:space="preserve">the list of collected historical images of defective and non-defective devices are used in training AI classifier </v>
       </c>
       <c r="E8" s="28" t="str">
         <f>'Step 1A - UC 1'!D14</f>
-        <v xml:space="preserve">if number of defective devices &gt; threshold </v>
+        <v xml:space="preserve">The trained model classifier are used in real time classification through camera to classify each product as eigher defective or non-defective and also measure its defective urgency. </v>
       </c>
       <c r="F8" s="28" t="str">
         <f>'Step 1A - UC 1'!E14</f>
-        <v>stop machine /line. The accuracy if very hight the machine/line will be stopped only if there are defectives</v>
+        <v xml:space="preserve">high defective productes thershold may stop or pause the production line. Git rid of the defective product. </v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15">
@@ -45739,7 +45749,7 @@
         <v>52</v>
       </c>
       <c r="D13" s="82" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -45748,7 +45758,7 @@
         <v>53</v>
       </c>
       <c r="D14" s="82" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15">
@@ -45756,7 +45766,7 @@
         <v>54</v>
       </c>
       <c r="D15" s="82" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="15">
@@ -45767,7 +45777,7 @@
         <v>56</v>
       </c>
       <c r="D17" s="81" t="s">
-        <v>295</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="15">
@@ -45775,7 +45785,7 @@
         <v>57</v>
       </c>
       <c r="D18" s="81" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="15">
@@ -45783,7 +45793,7 @@
         <v>58</v>
       </c>
       <c r="D19" s="81" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="15">
@@ -45791,7 +45801,7 @@
         <v>59</v>
       </c>
       <c r="D20" s="81" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="15">
@@ -45799,7 +45809,7 @@
         <v>60</v>
       </c>
       <c r="D21" s="81" t="s">
-        <v>299</v>
+        <v>283</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15">
@@ -45929,7 +45939,7 @@
         <v>52</v>
       </c>
       <c r="D13" s="82" t="s">
-        <v>300</v>
+        <v>284</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -45938,7 +45948,7 @@
         <v>53</v>
       </c>
       <c r="D14" s="82" t="s">
-        <v>301</v>
+        <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15">
@@ -45946,7 +45956,7 @@
         <v>54</v>
       </c>
       <c r="D15" s="82" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="15">
@@ -45957,7 +45967,7 @@
         <v>56</v>
       </c>
       <c r="D17" s="83" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="15">
@@ -45965,7 +45975,7 @@
         <v>57</v>
       </c>
       <c r="D18" s="83" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="15">
@@ -45973,7 +45983,7 @@
         <v>58</v>
       </c>
       <c r="D19" s="83" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="15">
@@ -45981,7 +45991,7 @@
         <v>59</v>
       </c>
       <c r="D20" s="83" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="15">
@@ -45989,7 +45999,7 @@
         <v>60</v>
       </c>
       <c r="D21" s="83" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15">

</xml_diff>

<commit_message>
updated Car Maintennce expectator use case
</commit_message>
<xml_diff>
--- a/01_project-steps-delivering-an-ml-ai-strategy.xlsx
+++ b/01_project-steps-delivering-an-ml-ai-strategy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDriveSysncOsa\OneDrive - Taibah University\DropBox\1440-1441 Second Semester\Udacity Reviewer\My own projects\ML Project\Github Repo\Delivering-an-ML-AI-Strategy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="221" documentId="13_ncr:1_{F6D73E04-F98F-4F45-82A3-AB2F1AC194F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3630EBB2-B9A1-48BC-885C-DB18A6645A3A}"/>
+  <xr:revisionPtr revIDLastSave="267" documentId="13_ncr:1_{F6D73E04-F98F-4F45-82A3-AB2F1AC194F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D7B12531-74D5-4EC1-B73B-2430131CD889}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="15" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIRECTIONS" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="333">
   <si>
     <t>Step 0: Choose Your Business Context</t>
   </si>
@@ -1297,33 +1297,6 @@
     <t>(Quality Control with Computer Vision )</t>
   </si>
   <si>
-    <t>(Optimal tax strategy predictor)</t>
-  </si>
-  <si>
-    <t>collecting tax codes</t>
-  </si>
-  <si>
-    <t>finding connections with organization tax policies</t>
-  </si>
-  <si>
-    <t>update policies</t>
-  </si>
-  <si>
-    <t>create tax strategy</t>
-  </si>
-  <si>
-    <t>tax codes are collected</t>
-  </si>
-  <si>
-    <t>generic predictors are used in accordance with the organization's ERP</t>
-  </si>
-  <si>
-    <t>tax codes are segmented using NLP</t>
-  </si>
-  <si>
-    <t>predict the best tax strategy</t>
-  </si>
-  <si>
     <t>(Car Detection of Customer ID)</t>
   </si>
   <si>
@@ -1376,30 +1349,6 @@
   </si>
   <si>
     <t> increased profits of the enterprise</t>
-  </si>
-  <si>
-    <t>https://www.jdsupra.com/legalnews/beyond-predictions-using-machine-59906/</t>
-  </si>
-  <si>
-    <t>https://turbotax.intuit.com/tax-tools/calculators/taxcaster/</t>
-  </si>
-  <si>
-    <t>https://www.mckinsey.com/industries/public-sector/our-insights/four-innovations-reshaping-tax-administration</t>
-  </si>
-  <si>
-    <t>tax automation</t>
-  </si>
-  <si>
-    <t>tax calculator with build in machine learning</t>
-  </si>
-  <si>
-    <t>reducing labor</t>
-  </si>
-  <si>
-    <t>accuracy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">automation leads to tax commitment </t>
   </si>
   <si>
     <t>https://ieeexplore.ieee.org/document/7613199</t>
@@ -1562,6 +1511,64 @@
   </si>
   <si>
     <t xml:space="preserve">defects are encountered </t>
+  </si>
+  <si>
+    <t>(Recruiting Screener)</t>
+  </si>
+  <si>
+    <t>https://ideal.com/ai-recruiting/</t>
+  </si>
+  <si>
+    <t>https://vervoe.com/blog/ai-recruitment/</t>
+  </si>
+  <si>
+    <t>https://ideal.com/resume-screening-tools/</t>
+  </si>
+  <si>
+    <t>Resume screening</t>
+  </si>
+  <si>
+    <t>AI for recruiting</t>
+  </si>
+  <si>
+    <t>HR helper</t>
+  </si>
+  <si>
+    <t>Candidate Assessment</t>
+  </si>
+  <si>
+    <t>Resume screening tool</t>
+  </si>
+  <si>
+    <t>collecting resumes
+- data from social media
+- data from linkedin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data is organized to put the candidates with sufficient skills needed, the candidate selection may need other criterias </t>
+  </si>
+  <si>
+    <t>Look for the candidate(s) with skills required and rank each one 
+- sort the candidates according to their rank 
+- select the top n candidates</t>
+  </si>
+  <si>
+    <t>contact the n candidates
+- make interview</t>
+  </si>
+  <si>
+    <t>collecting resumes 
+- label collected resumes, they maybe done be collecting resumes of current employer and rate them</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keywords are extracted from resumes.
+- NLA might be used to read resume and extract the candidate skill set. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">resumes are ranked using supervised learning classification model, each resume may be belonging to class A, B, C, D etc. </t>
+  </si>
+  <si>
+    <t>select top n candiates and start the hiring process.</t>
   </si>
 </sst>
 </file>
@@ -3434,7 +3441,7 @@
         <v>52</v>
       </c>
       <c r="D13" s="82" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -3443,7 +3450,7 @@
         <v>53</v>
       </c>
       <c r="D14" s="82" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15">
@@ -3451,7 +3458,7 @@
         <v>54</v>
       </c>
       <c r="D15" s="82" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="15">
@@ -3462,7 +3469,7 @@
         <v>56</v>
       </c>
       <c r="D17" s="83" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="15">
@@ -3470,7 +3477,7 @@
         <v>57</v>
       </c>
       <c r="D18" s="83" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="15">
@@ -3478,7 +3485,7 @@
         <v>58</v>
       </c>
       <c r="D19" s="83" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="15">
@@ -3486,7 +3493,7 @@
         <v>59</v>
       </c>
       <c r="D20" s="83" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="15">
@@ -3494,7 +3501,7 @@
         <v>60</v>
       </c>
       <c r="D21" s="83" t="s">
-        <v>290</v>
+        <v>273</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15">
@@ -3623,7 +3630,7 @@
         <v>52</v>
       </c>
       <c r="D13" s="82" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -3632,7 +3639,7 @@
         <v>53</v>
       </c>
       <c r="D14" s="82" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15">
@@ -3640,7 +3647,7 @@
         <v>54</v>
       </c>
       <c r="D15" s="82" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="15">
@@ -3651,7 +3658,7 @@
         <v>56</v>
       </c>
       <c r="D17" s="83" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="15">
@@ -3659,7 +3666,7 @@
         <v>57</v>
       </c>
       <c r="D18" s="81" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="15">
@@ -3667,7 +3674,7 @@
         <v>58</v>
       </c>
       <c r="D19" s="81" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="15">
@@ -3675,7 +3682,7 @@
         <v>59</v>
       </c>
       <c r="D20" s="81" t="s">
-        <v>297</v>
+        <v>280</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="15">
@@ -3683,7 +3690,7 @@
         <v>60</v>
       </c>
       <c r="D21" s="81" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15">
@@ -3814,7 +3821,7 @@
         <v>52</v>
       </c>
       <c r="D13" s="82" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -3823,7 +3830,7 @@
         <v>53</v>
       </c>
       <c r="D14" s="82" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15">
@@ -3831,7 +3838,7 @@
         <v>54</v>
       </c>
       <c r="D15" s="82" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="15">
@@ -3842,7 +3849,7 @@
         <v>56</v>
       </c>
       <c r="D17" s="81" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="15">
@@ -3850,7 +3857,7 @@
         <v>57</v>
       </c>
       <c r="D18" s="81" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="15">
@@ -3858,7 +3865,7 @@
         <v>58</v>
       </c>
       <c r="D19" s="81" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="15">
@@ -3866,7 +3873,7 @@
         <v>59</v>
       </c>
       <c r="D20" s="81" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="15">
@@ -3874,7 +3881,7 @@
         <v>60</v>
       </c>
       <c r="D21" s="81" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15">
@@ -3910,7 +3917,7 @@
   <dimension ref="A1:K1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -3959,7 +3966,7 @@
         <v>78</v>
       </c>
       <c r="K4" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
@@ -4059,7 +4066,7 @@
         <v>97</v>
       </c>
       <c r="K19" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="4:11" ht="15.75" customHeight="1">
@@ -4089,7 +4096,7 @@
         <v>102</v>
       </c>
       <c r="K24" s="44">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="4:11" ht="15">
@@ -7043,7 +7050,7 @@
   <dimension ref="A1:K1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -7067,7 +7074,7 @@
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="B2" s="39" t="str">
         <f>'Step 1A - UC 2'!B9</f>
-        <v>(Optimal tax strategy predictor)</v>
+        <v>(Recruiting Screener)</v>
       </c>
       <c r="C2" s="37"/>
       <c r="D2" s="37"/>
@@ -7076,7 +7083,8 @@
     <row r="3" spans="1:11" ht="15.75" customHeight="1">
       <c r="B3" s="41" t="str">
         <f>'Step 1A - UC 2'!B14</f>
-        <v>tax codes are collected</v>
+        <v>collecting resumes 
+- label collected resumes, they maybe done be collecting resumes of current employer and rate them</v>
       </c>
       <c r="D3" s="43" t="s">
         <v>79</v>
@@ -7091,7 +7099,7 @@
         <v>78</v>
       </c>
       <c r="K4" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
@@ -7132,7 +7140,7 @@
         <v>86</v>
       </c>
       <c r="K10" s="44">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
@@ -7173,7 +7181,7 @@
         <v>93</v>
       </c>
       <c r="K16" s="44">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="4:11" ht="15">
@@ -7191,7 +7199,7 @@
         <v>97</v>
       </c>
       <c r="K19" s="44">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="4:11" ht="15.75" customHeight="1">
@@ -7221,7 +7229,7 @@
         <v>102</v>
       </c>
       <c r="K24" s="44">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="4:11" ht="15">
@@ -10175,7 +10183,7 @@
   <dimension ref="A1:K1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -10265,7 +10273,7 @@
         <v>86</v>
       </c>
       <c r="K10" s="44">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
@@ -10324,7 +10332,7 @@
         <v>97</v>
       </c>
       <c r="K19" s="44">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="4:11" ht="15.75" customHeight="1">
@@ -10354,7 +10362,7 @@
         <v>102</v>
       </c>
       <c r="K24" s="44">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="4:11" ht="15.75" customHeight="1">
@@ -13315,7 +13323,7 @@
   <dimension ref="A1:K1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -13363,7 +13371,7 @@
         <v>78</v>
       </c>
       <c r="K4" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
@@ -13404,7 +13412,7 @@
         <v>86</v>
       </c>
       <c r="K10" s="44">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
@@ -13463,7 +13471,7 @@
         <v>97</v>
       </c>
       <c r="K19" s="44">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="4:11" ht="15.75" customHeight="1">
@@ -16447,7 +16455,7 @@
   <dimension ref="A1:K1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -16497,7 +16505,7 @@
         <v>78</v>
       </c>
       <c r="K4" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
@@ -16538,7 +16546,7 @@
         <v>86</v>
       </c>
       <c r="K10" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
@@ -16579,7 +16587,7 @@
         <v>93</v>
       </c>
       <c r="K16" s="44">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="4:11" ht="15">
@@ -16597,7 +16605,7 @@
         <v>97</v>
       </c>
       <c r="K19" s="44">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="4:11" ht="15.75" customHeight="1">
@@ -16627,7 +16635,7 @@
         <v>102</v>
       </c>
       <c r="K24" s="44">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="4:11" ht="15">
@@ -19630,7 +19638,7 @@
         <v>resolution</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="F4" s="43" t="s">
         <v>118</v>
@@ -19706,7 +19714,7 @@
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
       <c r="B2" s="91" t="str">
         <f>'Step 1A - UC 2'!B9</f>
-        <v>(Optimal tax strategy predictor)</v>
+        <v>(Recruiting Screener)</v>
       </c>
       <c r="C2" s="92"/>
       <c r="E2" s="43" t="s">
@@ -19716,11 +19724,12 @@
     <row r="3" spans="1:8" ht="15.75" customHeight="1">
       <c r="B3" s="47" t="str">
         <f>'Step 1A - UC 2'!C14</f>
-        <v>tax codes are segmented using NLP</v>
+        <v xml:space="preserve">keywords are extracted from resumes.
+- NLA might be used to read resume and extract the candidate skill set. </v>
       </c>
       <c r="C3" s="47" t="str">
         <f>'Step 1A - UC 2'!D14</f>
-        <v>generic predictors are used in accordance with the organization's ERP</v>
+        <v xml:space="preserve">resumes are ranked using supervised learning classification model, each resume may be belonging to class A, B, C, D etc. </v>
       </c>
       <c r="E3" s="48"/>
     </row>
@@ -19734,7 +19743,7 @@
         <v>resolution</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="F4" s="43" t="s">
         <v>118</v>
@@ -19750,7 +19759,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="F5" s="43" t="s">
         <v>119</v>
@@ -19954,7 +19963,7 @@
         <v>resolution</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="F4" s="43" t="s">
         <v>118</v>
@@ -19981,9 +19990,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1">
-      <c r="E7" s="44" t="s">
-        <v>307</v>
-      </c>
+      <c r="E7" s="44"/>
       <c r="F7" s="43" t="s">
         <v>121</v>
       </c>
@@ -20017,7 +20024,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -20080,7 +20087,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="F5" s="43" t="s">
         <v>119</v>
@@ -20127,7 +20134,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -20190,20 +20197,24 @@
         <v>0</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="F5" s="43" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1">
-      <c r="E6" s="44"/>
+      <c r="E6" s="50" t="s">
+        <v>290</v>
+      </c>
       <c r="F6" s="43" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1">
-      <c r="E7" s="44"/>
+      <c r="E7" s="50" t="s">
+        <v>290</v>
+      </c>
       <c r="F7" s="43" t="s">
         <v>121</v>
       </c>
@@ -20236,7 +20247,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
@@ -20460,7 +20471,7 @@
       <c r="B12" s="62"/>
       <c r="C12" s="62"/>
       <c r="D12" s="63" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="E12" s="64"/>
       <c r="F12" s="64"/>
@@ -21576,7 +21587,7 @@
       <c r="B108" s="64"/>
       <c r="C108" s="64"/>
       <c r="D108" s="63" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="E108" s="64"/>
       <c r="F108" s="64"/>
@@ -24640,7 +24651,7 @@
       <c r="B12" s="62"/>
       <c r="C12" s="62"/>
       <c r="D12" s="63" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="E12" s="64"/>
       <c r="F12" s="64"/>
@@ -25628,7 +25639,7 @@
       <c r="B96" s="64"/>
       <c r="C96" s="64"/>
       <c r="D96" s="63" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="E96" s="64"/>
       <c r="F96" s="64"/>
@@ -28714,7 +28725,7 @@
       <c r="B6" s="62"/>
       <c r="C6" s="62"/>
       <c r="D6" s="63" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="E6" s="64"/>
       <c r="F6" s="64"/>
@@ -30175,8 +30186,8 @@
   </sheetPr>
   <dimension ref="A1:E1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -30270,16 +30281,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="80" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
       <c r="C10" s="80" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
       <c r="D10" s="80" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
       <c r="E10" s="80" t="s">
-        <v>312</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15">
@@ -30323,16 +30334,16 @@
     </row>
     <row r="14" spans="1:5" ht="123.75" customHeight="1">
       <c r="B14" s="80" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
       <c r="C14" s="80" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
       <c r="D14" s="80" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
       <c r="E14" s="80" t="s">
-        <v>316</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15">
@@ -33309,7 +33320,7 @@
   <dimension ref="A1:AA1005"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -33414,7 +33425,7 @@
     </row>
     <row r="9" spans="1:27" ht="42" customHeight="1">
       <c r="B9" s="86" t="s">
-        <v>248</v>
+        <v>316</v>
       </c>
       <c r="C9" s="85"/>
       <c r="D9" s="85"/>
@@ -33442,21 +33453,21 @@
       <c r="Z9" s="24"/>
       <c r="AA9" s="24"/>
     </row>
-    <row r="10" spans="1:27" ht="36">
+    <row r="10" spans="1:27" ht="90">
       <c r="A10" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>249</v>
+        <v>325</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>250</v>
+        <v>326</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>251</v>
+        <v>327</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>252</v>
+        <v>328</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15">
@@ -33498,18 +33509,18 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="60" customHeight="1">
+    <row r="14" spans="1:27" ht="99" customHeight="1">
       <c r="B14" s="13" t="s">
-        <v>253</v>
+        <v>329</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>255</v>
+        <v>330</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>254</v>
+        <v>331</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>256</v>
+        <v>332</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="15">
@@ -36502,7 +36513,7 @@
     </row>
     <row r="9" spans="1:27" ht="34.5" customHeight="1">
       <c r="B9" s="86" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="C9" s="85"/>
       <c r="D9" s="85"/>
@@ -36535,16 +36546,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>322</v>
+        <v>305</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>323</v>
+        <v>306</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15">
@@ -36588,16 +36599,16 @@
     </row>
     <row r="14" spans="1:27" ht="84" customHeight="1">
       <c r="B14" s="13" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="15">
@@ -39590,7 +39601,7 @@
     </row>
     <row r="9" spans="1:27" ht="74.25" customHeight="1">
       <c r="B9" s="86" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C9" s="85"/>
       <c r="D9" s="85"/>
@@ -39623,16 +39634,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>332</v>
+        <v>315</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15">
@@ -39676,16 +39687,16 @@
     </row>
     <row r="14" spans="1:27" ht="35.25" customHeight="1">
       <c r="B14" s="13" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="15">
@@ -42678,7 +42689,7 @@
     </row>
     <row r="9" spans="1:27" ht="37.5" customHeight="1">
       <c r="B9" s="86" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C9" s="85"/>
       <c r="D9" s="85"/>
@@ -42711,16 +42722,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>325</v>
+        <v>308</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>326</v>
+        <v>309</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>327</v>
+        <v>310</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>328</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15">
@@ -42764,16 +42775,16 @@
     </row>
     <row r="14" spans="1:27" ht="107.25" customHeight="1">
       <c r="B14" s="13" t="s">
-        <v>329</v>
+        <v>312</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>330</v>
+        <v>313</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>328</v>
+        <v>311</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="15">
@@ -45756,7 +45767,7 @@
         <v>52</v>
       </c>
       <c r="D13" s="82" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -45765,7 +45776,7 @@
         <v>53</v>
       </c>
       <c r="D14" s="82" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15">
@@ -45773,7 +45784,7 @@
         <v>54</v>
       </c>
       <c r="D15" s="82" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="15">
@@ -45784,7 +45795,7 @@
         <v>56</v>
       </c>
       <c r="D17" s="81" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="15">
@@ -45792,7 +45803,7 @@
         <v>57</v>
       </c>
       <c r="D18" s="81" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="15">
@@ -45800,7 +45811,7 @@
         <v>58</v>
       </c>
       <c r="D19" s="81" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="15">
@@ -45808,7 +45819,7 @@
         <v>59</v>
       </c>
       <c r="D20" s="81" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="15">
@@ -45816,7 +45827,7 @@
         <v>60</v>
       </c>
       <c r="D21" s="81" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15">
@@ -45852,7 +45863,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -45893,7 +45904,7 @@
       <c r="B7" s="26"/>
       <c r="C7" s="90" t="str">
         <f>'Step 1A - UC 2'!B9</f>
-        <v>(Optimal tax strategy predictor)</v>
+        <v>(Recruiting Screener)</v>
       </c>
       <c r="D7" s="88"/>
       <c r="E7" s="88"/>
@@ -45905,19 +45916,21 @@
       </c>
       <c r="C8" s="28" t="str">
         <f>'Step 1A - UC 2'!B14</f>
-        <v>tax codes are collected</v>
+        <v>collecting resumes 
+- label collected resumes, they maybe done be collecting resumes of current employer and rate them</v>
       </c>
       <c r="D8" s="28" t="str">
         <f>'Step 1A - UC 2'!C14</f>
-        <v>tax codes are segmented using NLP</v>
+        <v xml:space="preserve">keywords are extracted from resumes.
+- NLA might be used to read resume and extract the candidate skill set. </v>
       </c>
       <c r="E8" s="28" t="str">
         <f>'Step 1A - UC 2'!D14</f>
-        <v>generic predictors are used in accordance with the organization's ERP</v>
+        <v xml:space="preserve">resumes are ranked using supervised learning classification model, each resume may be belonging to class A, B, C, D etc. </v>
       </c>
       <c r="F8" s="28" t="str">
         <f>'Step 1A - UC 2'!E14</f>
-        <v>predict the best tax strategy</v>
+        <v>select top n candiates and start the hiring process.</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15">
@@ -45946,7 +45959,7 @@
         <v>52</v>
       </c>
       <c r="D13" s="82" t="s">
-        <v>275</v>
+        <v>317</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -45955,7 +45968,7 @@
         <v>53</v>
       </c>
       <c r="D14" s="82" t="s">
-        <v>276</v>
+        <v>318</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15">
@@ -45963,7 +45976,7 @@
         <v>54</v>
       </c>
       <c r="D15" s="82" t="s">
-        <v>277</v>
+        <v>319</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="15">
@@ -45974,7 +45987,7 @@
         <v>56</v>
       </c>
       <c r="D17" s="83" t="s">
-        <v>278</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="15">
@@ -45982,7 +45995,7 @@
         <v>57</v>
       </c>
       <c r="D18" s="83" t="s">
-        <v>279</v>
+        <v>321</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="15">
@@ -45990,7 +46003,7 @@
         <v>58</v>
       </c>
       <c r="D19" s="83" t="s">
-        <v>280</v>
+        <v>322</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="15">
@@ -45998,7 +46011,7 @@
         <v>59</v>
       </c>
       <c r="D20" s="83" t="s">
-        <v>281</v>
+        <v>323</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="15">
@@ -46006,7 +46019,7 @@
         <v>60</v>
       </c>
       <c r="D21" s="83" t="s">
-        <v>282</v>
+        <v>324</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15">
@@ -46024,9 +46037,9 @@
     <mergeCell ref="C7:F7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D13" r:id="rId1" xr:uid="{7EC0DE22-DE50-40B7-96D9-B4EDEC7B66D6}"/>
-    <hyperlink ref="D14" r:id="rId2" xr:uid="{D0330F90-332C-47EB-8D34-6D433EFD1CB7}"/>
-    <hyperlink ref="D15" r:id="rId3" xr:uid="{D2D7B9A9-0918-4079-848A-9860258DE305}"/>
+    <hyperlink ref="D13" r:id="rId1" xr:uid="{7909738B-2A28-46ED-B389-66EA32B99938}"/>
+    <hyperlink ref="D14" r:id="rId2" xr:uid="{344FD382-4577-44B4-995A-772B6C5C3D1F}"/>
+    <hyperlink ref="D15" r:id="rId3" xr:uid="{51A63258-1B45-462C-B114-F2EB63294504}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>